<commit_message>
fix raw data brandenburg
</commit_message>
<xml_diff>
--- a/data/municipal_elections/raw/brandenburg/brandenburg_1993.xlsx
+++ b/data/municipal_elections/raw/brandenburg/brandenburg_1993.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flosic/Documents/GitHub/german_election_data/data/municipal_elections/raw/brandenburg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C624B4B1-F669-5E40-8317-1ED894E28DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C826E47B-C6EF-6141-8475-93A2BD6C6F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4120" yWindow="-23280" windowWidth="30240" windowHeight="17940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ergebnis" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3412" uniqueCount="2997">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3412" uniqueCount="2999">
   <si>
     <t>060 000</t>
   </si>
@@ -9016,6 +9016,12 @@
   </si>
   <si>
     <t>Wahlberechtigte</t>
+  </si>
+  <si>
+    <t>067 452</t>
+  </si>
+  <si>
+    <t>073 636</t>
   </si>
 </sst>
 </file>
@@ -9090,7 +9096,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -9111,13 +9117,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9400,8 +9405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BMV74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="AHL1" workbookViewId="0">
+      <selection activeCell="AHO13" sqref="AHO13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -9436,10 +9441,10 @@
       </c>
     </row>
     <row r="2" spans="1:1712" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="3" t="s">
         <v>2988</v>
       </c>
-      <c r="B2" s="12"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -12084,7 +12089,7 @@
         <v>2992</v>
       </c>
       <c r="AGZ2" s="2" t="s">
-        <v>1626</v>
+        <v>2997</v>
       </c>
       <c r="AHA2" s="2" t="s">
         <v>1591</v>
@@ -14556,7 +14561,7 @@
         <v>2891</v>
       </c>
       <c r="BMR2" s="2" t="s">
-        <v>2854</v>
+        <v>2998</v>
       </c>
       <c r="BMS2" s="2" t="s">
         <v>2894</v>
@@ -96888,14 +96893,14 @@
       <c r="ZG35" s="9"/>
     </row>
     <row r="45" spans="680:683" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="ZD45" s="10"/>
-      <c r="ZE45" s="10"/>
-      <c r="ZF45" s="10"/>
+      <c r="ZD45" s="11"/>
+      <c r="ZE45" s="11"/>
+      <c r="ZF45" s="11"/>
     </row>
     <row r="67" spans="115:117" x14ac:dyDescent="0.2">
-      <c r="DK67" s="11"/>
-      <c r="DL67" s="11"/>
-      <c r="DM67" s="11"/>
+      <c r="DK67" s="10"/>
+      <c r="DL67" s="10"/>
+      <c r="DM67" s="10"/>
     </row>
     <row r="72" spans="115:117" x14ac:dyDescent="0.2">
       <c r="DM72" s="5"/>

</xml_diff>

<commit_message>
Vincent's updates for R&R
</commit_message>
<xml_diff>
--- a/data/municipal_elections/raw/brandenburg/brandenburg_1993.xlsx
+++ b/data/municipal_elections/raw/brandenburg/brandenburg_1993.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flosic/Documents/GitHub/german_election_data/data/municipal_elections/raw/brandenburg/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincentheddesheimer/Documents/GitHub/german_election_data/data/municipal_elections/raw/brandenburg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260C27A4-6650-FD4E-AF1D-39BEAD7F0295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537AD5B3-9FD1-5142-83F9-779E256A6366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2080" yWindow="-22360" windowWidth="30240" windowHeight="17940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ergebnis" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3388" uniqueCount="2980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3387" uniqueCount="2979">
   <si>
     <t>060 004</t>
   </si>
@@ -8683,9 +8683,6 @@
   </si>
   <si>
     <t>073 480</t>
-  </si>
-  <si>
-    <t>668C</t>
   </si>
   <si>
     <t>58,51</t>
@@ -9068,7 +9065,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -9348,8 +9345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BML74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AWT1048576"/>
+    <sheetView tabSelected="1" topLeftCell="TY1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="UL21" sqref="UL21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -9381,25 +9378,25 @@
   <sheetData>
     <row r="1" spans="1:1702" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>2965</v>
+        <v>2964</v>
       </c>
     </row>
     <row r="2" spans="1:1702" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>2964</v>
+        <v>2963</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="1" t="s">
+        <v>2976</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2975</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>2977</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>2976</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>2978</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>2979</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>0</v>
@@ -9435,7 +9432,7 @@
         <v>52</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>2975</v>
+        <v>2974</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>53</v>
@@ -9789,7 +9786,7 @@
         <v>260</v>
       </c>
       <c r="EF2" s="2" t="s">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="EG2" s="2" t="s">
         <v>261</v>
@@ -11169,7 +11166,7 @@
         <v>1093</v>
       </c>
       <c r="VX2" s="2" t="s">
-        <v>2969</v>
+        <v>2968</v>
       </c>
       <c r="VY2" s="2" t="s">
         <v>1094</v>
@@ -11766,7 +11763,7 @@
         <v>1435</v>
       </c>
       <c r="ADO2" s="2" t="s">
-        <v>2971</v>
+        <v>2970</v>
       </c>
       <c r="ADP2" s="2" t="s">
         <v>1436</v>
@@ -12018,10 +12015,10 @@
         <v>1567</v>
       </c>
       <c r="AGU2" s="2" t="s">
-        <v>2968</v>
+        <v>2967</v>
       </c>
       <c r="AGV2" s="2" t="s">
-        <v>2973</v>
+        <v>2972</v>
       </c>
       <c r="AGW2" s="2" t="s">
         <v>1576</v>
@@ -12210,7 +12207,7 @@
         <v>1665</v>
       </c>
       <c r="AJG2" s="2" t="s">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="AJH2" s="2" t="s">
         <v>1666</v>
@@ -12822,7 +12819,7 @@
         <v>1990</v>
       </c>
       <c r="ARC2" s="2" t="s">
-        <v>2970</v>
+        <v>2969</v>
       </c>
       <c r="ARD2" s="2" t="s">
         <v>1991</v>
@@ -14475,7 +14472,7 @@
         <v>2867</v>
       </c>
       <c r="BMH2" s="2" t="s">
-        <v>2974</v>
+        <v>2973</v>
       </c>
       <c r="BMI2" s="2" t="s">
         <v>2870</v>
@@ -14492,7 +14489,7 @@
     </row>
     <row r="3" spans="1:1702" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>2972</v>
+        <v>2971</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>34</v>
@@ -16094,8 +16091,8 @@
       <c r="UC3" s="2">
         <v>238</v>
       </c>
-      <c r="UD3" s="2" t="s">
-        <v>2886</v>
+      <c r="UD3" s="2">
+        <v>6680</v>
       </c>
       <c r="UE3" s="2">
         <v>435</v>
@@ -24494,10 +24491,10 @@
         <v>43</v>
       </c>
       <c r="O5" s="2" t="s">
+        <v>2886</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>2887</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>2888</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>44</v>
@@ -24521,16 +24518,16 @@
         <v>58</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>2889</v>
+        <v>2888</v>
       </c>
       <c r="Y5" s="2" t="s">
         <v>59</v>
       </c>
       <c r="Z5" s="2" t="s">
+        <v>2889</v>
+      </c>
+      <c r="AA5" s="2" t="s">
         <v>2890</v>
-      </c>
-      <c r="AA5" s="2" t="s">
-        <v>2891</v>
       </c>
       <c r="AB5" s="2" t="s">
         <v>60</v>
@@ -24634,7 +24631,7 @@
         <v>137</v>
       </c>
       <c r="BK5" s="2" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
       <c r="BL5" s="2" t="s">
         <v>138</v>
@@ -24699,11 +24696,11 @@
         <v>542</v>
       </c>
       <c r="CH5" s="2" t="s">
-        <v>2893</v>
+        <v>2892</v>
       </c>
       <c r="CI5" s="2"/>
       <c r="CJ5" s="2" t="s">
-        <v>2894</v>
+        <v>2893</v>
       </c>
       <c r="CK5" s="2" t="s">
         <v>179</v>
@@ -24718,7 +24715,7 @@
         <v>181</v>
       </c>
       <c r="CO5" s="2" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="CP5" s="2" t="s">
         <v>182</v>
@@ -24862,7 +24859,7 @@
         <v>272</v>
       </c>
       <c r="EM5" s="2" t="s">
-        <v>2896</v>
+        <v>2895</v>
       </c>
       <c r="EN5" s="2" t="s">
         <v>281</v>
@@ -24905,7 +24902,7 @@
         <v>300</v>
       </c>
       <c r="FB5" s="2" t="s">
-        <v>2897</v>
+        <v>2896</v>
       </c>
       <c r="FC5" s="2" t="s">
         <v>309</v>
@@ -24999,7 +24996,7 @@
         <v>360</v>
       </c>
       <c r="GH5" s="2" t="s">
-        <v>2898</v>
+        <v>2897</v>
       </c>
       <c r="GI5" s="2" t="s">
         <v>369</v>
@@ -25045,7 +25042,7 @@
         <v>390</v>
       </c>
       <c r="GX5" s="2" t="s">
-        <v>2899</v>
+        <v>2898</v>
       </c>
       <c r="GY5" s="2" t="s">
         <v>399</v>
@@ -25134,7 +25131,7 @@
         <v>451</v>
       </c>
       <c r="IC5" s="2" t="s">
-        <v>2900</v>
+        <v>2899</v>
       </c>
       <c r="ID5" s="2" t="s">
         <v>452</v>
@@ -25216,7 +25213,7 @@
         <v>500</v>
       </c>
       <c r="JE5" s="2" t="s">
-        <v>2901</v>
+        <v>2900</v>
       </c>
       <c r="JF5" s="2" t="s">
         <v>509</v>
@@ -25246,7 +25243,7 @@
         <v>522</v>
       </c>
       <c r="JO5" s="2" t="s">
-        <v>2902</v>
+        <v>2901</v>
       </c>
       <c r="JP5" s="2" t="s">
         <v>523</v>
@@ -25264,7 +25261,7 @@
         <v>527</v>
       </c>
       <c r="JU5" s="2" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
       <c r="JV5" s="2" t="s">
         <v>537</v>
@@ -25340,7 +25337,7 @@
         <v>583</v>
       </c>
       <c r="KU5" s="2" t="s">
-        <v>2904</v>
+        <v>2903</v>
       </c>
       <c r="KV5" s="2" t="s">
         <v>282</v>
@@ -25364,7 +25361,7 @@
         <v>67.22</v>
       </c>
       <c r="LC5" s="2" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="LD5" s="2" t="s">
         <v>597</v>
@@ -25397,7 +25394,7 @@
         <v>614</v>
       </c>
       <c r="LN5" s="2" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
       <c r="LO5" s="2" t="s">
         <v>615</v>
@@ -25469,7 +25466,7 @@
         <v>660</v>
       </c>
       <c r="ML5" s="2" t="s">
-        <v>2890</v>
+        <v>2889</v>
       </c>
       <c r="MM5" s="2" t="s">
         <v>661</v>
@@ -25550,7 +25547,7 @@
         <v>706</v>
       </c>
       <c r="NM5" s="2" t="s">
-        <v>2907</v>
+        <v>2906</v>
       </c>
       <c r="NN5" s="2" t="s">
         <v>717</v>
@@ -25605,7 +25602,7 @@
         <v>747</v>
       </c>
       <c r="OF5" s="2" t="s">
-        <v>2908</v>
+        <v>2907</v>
       </c>
       <c r="OG5" s="2" t="s">
         <v>748</v>
@@ -25709,7 +25706,7 @@
         <v>809</v>
       </c>
       <c r="PP5" s="2" t="s">
-        <v>2909</v>
+        <v>2908</v>
       </c>
       <c r="PQ5" s="2" t="s">
         <v>818</v>
@@ -25778,7 +25775,7 @@
         <v>2265</v>
       </c>
       <c r="QM5" s="2" t="s">
-        <v>2910</v>
+        <v>2909</v>
       </c>
       <c r="QN5" s="2" t="s">
         <v>859</v>
@@ -25793,10 +25790,10 @@
         <v>860</v>
       </c>
       <c r="QR5" s="2" t="s">
+        <v>2910</v>
+      </c>
+      <c r="QS5" s="2" t="s">
         <v>2911</v>
-      </c>
-      <c r="QS5" s="2" t="s">
-        <v>2912</v>
       </c>
       <c r="QT5" s="2" t="s">
         <v>795</v>
@@ -25818,7 +25815,7 @@
         <v>874</v>
       </c>
       <c r="RA5" s="2" t="s">
-        <v>2913</v>
+        <v>2912</v>
       </c>
       <c r="RB5" s="2" t="s">
         <v>875</v>
@@ -25894,7 +25891,7 @@
         <v>922</v>
       </c>
       <c r="SA5" s="2" t="s">
-        <v>2914</v>
+        <v>2913</v>
       </c>
       <c r="SB5" s="2" t="s">
         <v>931</v>
@@ -25909,7 +25906,7 @@
         <v>934</v>
       </c>
       <c r="SF5" s="2" t="s">
-        <v>2913</v>
+        <v>2912</v>
       </c>
       <c r="SG5" s="2" t="s">
         <v>935</v>
@@ -25976,7 +25973,7 @@
         <v>974</v>
       </c>
       <c r="TC5" s="2" t="s">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="TD5" s="2" t="s">
         <v>975</v>
@@ -26022,7 +26019,7 @@
         <v>736</v>
       </c>
       <c r="TS5" s="2" t="s">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="TT5" s="2" t="s">
         <v>750</v>
@@ -26100,7 +26097,7 @@
         <v>1044</v>
       </c>
       <c r="US5" s="2" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="UT5" s="2" t="s">
         <v>840</v>
@@ -26124,7 +26121,7 @@
         <v>1056</v>
       </c>
       <c r="VA5" s="2" t="s">
-        <v>2918</v>
+        <v>2917</v>
       </c>
       <c r="VB5" s="2" t="s">
         <v>1057</v>
@@ -26235,7 +26232,7 @@
         <v>1125</v>
       </c>
       <c r="WL5" s="2" t="s">
-        <v>2919</v>
+        <v>2918</v>
       </c>
       <c r="WM5" s="2" t="s">
         <v>1126</v>
@@ -26247,7 +26244,7 @@
         <v>1127</v>
       </c>
       <c r="WP5" s="2" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="WQ5" s="2" t="s">
         <v>1136</v>
@@ -26314,10 +26311,10 @@
         <v>1170</v>
       </c>
       <c r="XM5" s="2" t="s">
+        <v>2919</v>
+      </c>
+      <c r="XN5" s="2" t="s">
         <v>2920</v>
-      </c>
-      <c r="XN5" s="2" t="s">
-        <v>2921</v>
       </c>
       <c r="XO5" s="2" t="s">
         <v>1179</v>
@@ -26475,7 +26472,7 @@
         <v>1274</v>
       </c>
       <c r="ZP5" s="2" t="s">
-        <v>2922</v>
+        <v>2921</v>
       </c>
       <c r="ZQ5" s="2" t="s">
         <v>1275</v>
@@ -26484,7 +26481,7 @@
         <v>1276</v>
       </c>
       <c r="ZS5" s="2" t="s">
-        <v>2923</v>
+        <v>2922</v>
       </c>
       <c r="ZT5" s="2" t="s">
         <v>1277</v>
@@ -26493,7 +26490,7 @@
         <v>1278</v>
       </c>
       <c r="ZV5" s="2" t="s">
-        <v>2924</v>
+        <v>2923</v>
       </c>
       <c r="ZW5" s="2" t="s">
         <v>1287</v>
@@ -26535,7 +26532,7 @@
         <v>1303</v>
       </c>
       <c r="AAJ5" s="2" t="s">
-        <v>2925</v>
+        <v>2924</v>
       </c>
       <c r="AAK5" s="2" t="s">
         <v>1304</v>
@@ -26623,7 +26620,7 @@
         <v>1357</v>
       </c>
       <c r="ABN5" s="2" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="ABO5" s="2" t="s">
         <v>1358</v>
@@ -26661,7 +26658,7 @@
         <v>1381</v>
       </c>
       <c r="ACB5" s="2" t="s">
-        <v>2927</v>
+        <v>2926</v>
       </c>
       <c r="ACC5" s="2" t="s">
         <v>1382</v>
@@ -26704,7 +26701,7 @@
         <v>1402</v>
       </c>
       <c r="ACQ5" s="2" t="s">
-        <v>2928</v>
+        <v>2927</v>
       </c>
       <c r="ACR5" s="2" t="s">
         <v>69</v>
@@ -26737,7 +26734,7 @@
         <v>574</v>
       </c>
       <c r="ADB5" s="2" t="s">
-        <v>2929</v>
+        <v>2928</v>
       </c>
       <c r="ADC5" s="2" t="s">
         <v>1425</v>
@@ -26762,7 +26759,7 @@
       </c>
       <c r="ADJ5" s="2"/>
       <c r="ADK5" s="2" t="s">
-        <v>2930</v>
+        <v>2929</v>
       </c>
       <c r="ADL5" s="2" t="s">
         <v>484</v>
@@ -26808,7 +26805,7 @@
         <v>1456</v>
       </c>
       <c r="AEA5" s="2" t="s">
-        <v>2931</v>
+        <v>2930</v>
       </c>
       <c r="AEB5" s="2" t="s">
         <v>1465</v>
@@ -26905,10 +26902,10 @@
         <v>618</v>
       </c>
       <c r="AFH5" s="2" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AFI5" s="2" t="s">
         <v>2932</v>
-      </c>
-      <c r="AFI5" s="2" t="s">
-        <v>2933</v>
       </c>
       <c r="AFJ5" s="2" t="s">
         <v>1522</v>
@@ -26987,7 +26984,7 @@
         <v>1559</v>
       </c>
       <c r="AGL5" s="2" t="s">
-        <v>2934</v>
+        <v>2933</v>
       </c>
       <c r="AGM5" s="2" t="s">
         <v>1568</v>
@@ -27041,7 +27038,7 @@
         <v>1302</v>
       </c>
       <c r="AHF5" s="2" t="s">
-        <v>2935</v>
+        <v>2934</v>
       </c>
       <c r="AHG5" s="2" t="s">
         <v>1594</v>
@@ -27120,7 +27117,7 @@
         <v>1634</v>
       </c>
       <c r="AII5" s="2" t="s">
-        <v>2936</v>
+        <v>2935</v>
       </c>
       <c r="AIJ5" s="2" t="s">
         <v>1635</v>
@@ -27141,7 +27138,7 @@
         <v>1645</v>
       </c>
       <c r="AIP5" s="2" t="s">
-        <v>2937</v>
+        <v>2936</v>
       </c>
       <c r="AIQ5" s="2" t="s">
         <v>1214</v>
@@ -27171,7 +27168,7 @@
         <v>989</v>
       </c>
       <c r="AIZ5" s="2" t="s">
-        <v>2938</v>
+        <v>2937</v>
       </c>
       <c r="AJA5" s="2" t="s">
         <v>1667</v>
@@ -27186,7 +27183,7 @@
         <v>1670</v>
       </c>
       <c r="AJE5" s="2" t="s">
-        <v>2939</v>
+        <v>2938</v>
       </c>
       <c r="AJF5" s="2" t="s">
         <v>1671</v>
@@ -27237,13 +27234,13 @@
         <v>1696</v>
       </c>
       <c r="AJV5" s="3" t="s">
+        <v>2939</v>
+      </c>
+      <c r="AJW5" s="3" t="s">
+        <v>2962</v>
+      </c>
+      <c r="AJX5" s="3" t="s">
         <v>2940</v>
-      </c>
-      <c r="AJW5" s="3" t="s">
-        <v>2963</v>
-      </c>
-      <c r="AJX5" s="3" t="s">
-        <v>2941</v>
       </c>
       <c r="AJY5" s="2" t="s">
         <v>822</v>
@@ -27337,7 +27334,7 @@
         <v>1026</v>
       </c>
       <c r="ALD5" s="2" t="s">
-        <v>2942</v>
+        <v>2941</v>
       </c>
       <c r="ALE5" s="2" t="s">
         <v>1751</v>
@@ -27478,7 +27475,7 @@
         <v>1265</v>
       </c>
       <c r="AMY5" s="2" t="s">
-        <v>2943</v>
+        <v>2942</v>
       </c>
       <c r="AMZ5" s="2" t="s">
         <v>329</v>
@@ -27526,7 +27523,7 @@
         <v>386</v>
       </c>
       <c r="ANO5" s="2" t="s">
-        <v>2944</v>
+        <v>2943</v>
       </c>
       <c r="ANP5" s="2" t="s">
         <v>706</v>
@@ -27586,7 +27583,7 @@
         <v>1635</v>
       </c>
       <c r="AOI5" s="2" t="s">
-        <v>2904</v>
+        <v>2903</v>
       </c>
       <c r="AOJ5" s="2" t="s">
         <v>1429</v>
@@ -27637,7 +27634,7 @@
         <v>935</v>
       </c>
       <c r="AOZ5" s="2" t="s">
-        <v>2945</v>
+        <v>2944</v>
       </c>
       <c r="APA5" s="2" t="s">
         <v>1904</v>
@@ -27731,7 +27728,7 @@
         <v>1961</v>
       </c>
       <c r="AQF5" s="2" t="s">
-        <v>2946</v>
+        <v>2945</v>
       </c>
       <c r="AQG5" s="2" t="s">
         <v>1962</v>
@@ -27841,7 +27838,7 @@
         <v>2025</v>
       </c>
       <c r="ARR5" s="2" t="s">
-        <v>2947</v>
+        <v>2946</v>
       </c>
       <c r="ARS5" s="2" t="s">
         <v>2051</v>
@@ -27871,7 +27868,7 @@
         <v>2039</v>
       </c>
       <c r="ASB5" s="2" t="s">
-        <v>2948</v>
+        <v>2947</v>
       </c>
       <c r="ASC5" s="2" t="s">
         <v>2040</v>
@@ -27928,7 +27925,7 @@
         <v>2068</v>
       </c>
       <c r="ASU5" s="2" t="s">
-        <v>2949</v>
+        <v>2948</v>
       </c>
       <c r="ASV5" s="2" t="s">
         <v>2078</v>
@@ -28093,7 +28090,7 @@
         <v>2163</v>
       </c>
       <c r="AUX5" s="2" t="s">
-        <v>2950</v>
+        <v>2949</v>
       </c>
       <c r="AUY5" s="2" t="s">
         <v>2172</v>
@@ -28303,7 +28300,7 @@
         <v>2279</v>
       </c>
       <c r="AXP5" s="2" t="s">
-        <v>2951</v>
+        <v>2950</v>
       </c>
       <c r="AXQ5" s="2" t="s">
         <v>467</v>
@@ -28618,7 +28615,7 @@
         <v>2448</v>
       </c>
       <c r="BBU5" s="2" t="s">
-        <v>2952</v>
+        <v>2951</v>
       </c>
       <c r="BBV5" s="2" t="s">
         <v>36</v>
@@ -28642,7 +28639,7 @@
         <v>94</v>
       </c>
       <c r="BCC5" s="2" t="s">
-        <v>2953</v>
+        <v>2952</v>
       </c>
       <c r="BCD5" s="2" t="s">
         <v>2461</v>
@@ -28666,7 +28663,7 @@
         <v>2472</v>
       </c>
       <c r="BCK5" s="2" t="s">
-        <v>2954</v>
+        <v>2953</v>
       </c>
       <c r="BCL5" s="2" t="s">
         <v>2473</v>
@@ -28767,7 +28764,7 @@
       <c r="BDR5" s="3"/>
       <c r="BDS5" s="3"/>
       <c r="BDT5" s="2" t="s">
-        <v>2955</v>
+        <v>2954</v>
       </c>
       <c r="BDU5" s="2" t="s">
         <v>779</v>
@@ -29045,7 +29042,7 @@
         <v>2675</v>
       </c>
       <c r="BHJ5" s="2" t="s">
-        <v>2956</v>
+        <v>2955</v>
       </c>
       <c r="BHK5" s="2" t="s">
         <v>2684</v>
@@ -29126,7 +29123,7 @@
         <v>2722</v>
       </c>
       <c r="BIK5" s="2" t="s">
-        <v>2957</v>
+        <v>2956</v>
       </c>
       <c r="BIL5" s="2" t="s">
         <v>2723</v>
@@ -29163,7 +29160,7 @@
         <v>418</v>
       </c>
       <c r="BIX5" s="2" t="s">
-        <v>2958</v>
+        <v>2957</v>
       </c>
       <c r="BIY5" s="2" t="s">
         <v>112</v>
@@ -29216,7 +29213,7 @@
       </c>
       <c r="BJP5" s="3"/>
       <c r="BJQ5" s="3" t="s">
-        <v>2959</v>
+        <v>2958</v>
       </c>
       <c r="BJR5" s="3" t="s">
         <v>2770</v>
@@ -29277,7 +29274,7 @@
         <v>2796</v>
       </c>
       <c r="BKL5" s="2" t="s">
-        <v>2960</v>
+        <v>2959</v>
       </c>
       <c r="BKM5" s="2" t="s">
         <v>2805</v>
@@ -44759,7 +44756,7 @@
         <v>84</v>
       </c>
       <c r="ND9" s="2" t="s">
-        <v>2961</v>
+        <v>2960</v>
       </c>
       <c r="NE9" s="2">
         <v>121</v>
@@ -88617,7 +88614,7 @@
         <v>1657</v>
       </c>
       <c r="ACT28" s="2" t="s">
-        <v>2962</v>
+        <v>2961</v>
       </c>
       <c r="ACU28" s="2"/>
       <c r="ACV28" s="2">

</xml_diff>